<commit_message>
EEG and nirs processing 1-23
</commit_message>
<xml_diff>
--- a/ANALYSIS SCRIPTS/channelsremoved.xlsx
+++ b/ANALYSIS SCRIPTS/channelsremoved.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="26" uniqueCount="19">
   <si>
     <t>NDARVX375BR6</t>
   </si>
@@ -53,11 +53,29 @@
   <si>
     <t>NDARVX375BR6</t>
   </si>
+  <si>
+    <t>NDARFV472HU7</t>
+  </si>
+  <si>
+    <t>NDARDC882NK4</t>
+  </si>
+  <si>
+    <t>NDARWB491KR3</t>
+  </si>
+  <si>
+    <t>NDARNL224RR9</t>
+  </si>
+  <si>
+    <t>NDARTT639AB1</t>
+  </si>
+  <si>
+    <t>NDARAZC45TW3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -107,8 +125,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="true"/>
-    <col min="2" max="2" width="2.15625" customWidth="true"/>
+    <col min="1" max="1" width="15.5703125" customWidth="true"/>
+    <col min="2" max="2" width="2.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -137,10 +155,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>